<commit_message>
Results from hybrid goal GA. Completed personal revison of SCOUt chapter.
</commit_message>
<xml_diff>
--- a/app/src/resources/ga-output/FindHumanLongRun/AverageFitnessVSTrainingIterations.xlsx
+++ b/app/src/resources/ga-output/FindHumanLongRun/AverageFitnessVSTrainingIterations.xlsx
@@ -3,29 +3,43 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C52C68-38E5-4EFA-B003-3240524AD430}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD20560-E044-4E1A-A353-1AAC3125A604}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>Average Fitness (Total Population)</t>
   </si>
   <si>
     <t>Average Fitness (Survivors)</t>
+  </si>
+  <si>
+    <t>Best Fitness</t>
+  </si>
+  <si>
+    <t>Best - Avg (Total Pop)</t>
+  </si>
+  <si>
+    <t>Best - Avg (Survivors)</t>
   </si>
 </sst>
 </file>
@@ -318,7 +332,391 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-24BF-4548-8AF1-2A7B2D25A593}"/>
+              <c16:uniqueId val="{00000000-F747-4565-AAAF-A7A5B0CDD611}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average Fitness (Survivors)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0.38023970761584802</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.45404853731502798</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.467551227227267</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.51580979418741002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.41041012997057802</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.45116237284016297</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.44053303734420801</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.45624399901880902</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.44017095324546601</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.43473856927003002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.446943342171707</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.44207149596212603</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.469899142097221</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.46846518303503398</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.42811127272982802</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.40866831313565499</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.45140650562437701</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.46756664380812002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.411241231291336</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.41742014532934102</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.430316903453132</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.482932282024571</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.47260827673611699</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.51180332990777599</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.489120466691017</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.46452647384373602</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.44376172228856098</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.460052217037696</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.39913249294169501</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.48736040310893602</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.44098937508365799</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.468838440376317</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.45572206176956698</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.423607965520926</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.466192529402921</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.47828012851038099</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.52057572179401201</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.41056632111063202</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.43630146557682797</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.446945851211624</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.457451915293831</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.48583065415085702</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.38334724327005698</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.40158398407027701</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.49157305190433698</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.420605034401628</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.45853497471309401</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.43134459522479002</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.45222270476099302</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.43415426904600302</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F747-4565-AAAF-A7A5B0CDD611}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Best Fitness</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.77</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F747-4565-AAAF-A7A5B0CDD611}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -331,11 +729,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="491444944"/>
-        <c:axId val="491445272"/>
+        <c:axId val="499521368"/>
+        <c:axId val="499521696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="491444944"/>
+        <c:axId val="499521368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -377,7 +775,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="491445272"/>
+        <c:crossAx val="499521696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -385,7 +783,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="491445272"/>
+        <c:axId val="499521696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -436,7 +834,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="491444944"/>
+        <c:crossAx val="499521368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -448,6 +846,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -547,11 +976,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>Sheet1!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Average Fitness (Survivors)</c:v>
+                  <c:v>Best - Avg (Total Pop)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -570,159 +999,159 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$51</c:f>
+              <c:f>Sheet1!$E$2:$E$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>0.38023970761584802</c:v>
+                  <c:v>0.30843195716054006</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.45404853731502798</c:v>
+                  <c:v>0.28977854931091496</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.467551227227267</c:v>
+                  <c:v>0.33495126897699301</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.51580979418741002</c:v>
+                  <c:v>0.32361658899858897</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.41041012997057802</c:v>
+                  <c:v>0.30718129235526898</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.45116237284016297</c:v>
+                  <c:v>0.39698548670158906</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.44053303734420801</c:v>
+                  <c:v>0.27780583486598398</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.45624399901880902</c:v>
+                  <c:v>0.32222916707365401</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.44017095324546601</c:v>
+                  <c:v>0.37442465263558705</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.43473856927003002</c:v>
+                  <c:v>0.27828453322417496</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.446943342171707</c:v>
+                  <c:v>0.30062206188555601</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.44207149596212603</c:v>
+                  <c:v>0.35792400402212404</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.469899142097221</c:v>
+                  <c:v>0.31150674669685202</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.46846518303503398</c:v>
+                  <c:v>0.32074844218510101</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.42811127272982802</c:v>
+                  <c:v>0.28213171561783795</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.40866831313565499</c:v>
+                  <c:v>0.32086095198671893</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.45140650562437701</c:v>
+                  <c:v>0.38500641747174208</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.46756664380812002</c:v>
+                  <c:v>0.38927992588496496</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.411241231291336</c:v>
+                  <c:v>0.27870223870674005</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.41742014532934102</c:v>
+                  <c:v>0.40612436622715603</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.430316903453132</c:v>
+                  <c:v>0.31813268976243797</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.482932282024571</c:v>
+                  <c:v>0.27723597835207398</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.47260827673611699</c:v>
+                  <c:v>0.28573779994790099</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.51180332990777599</c:v>
+                  <c:v>0.27946463770991803</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.489120466691017</c:v>
+                  <c:v>0.31521636280234805</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.46452647384373602</c:v>
+                  <c:v>0.340958684481528</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.44376172228856098</c:v>
+                  <c:v>0.34032969469495999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.460052217037696</c:v>
+                  <c:v>0.29273667537467501</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.39913249294169501</c:v>
+                  <c:v>0.31709896617739497</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.48736040310893602</c:v>
+                  <c:v>0.38508341090866</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.44098937508365799</c:v>
+                  <c:v>0.30962216911967499</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.468838440376317</c:v>
+                  <c:v>0.34597980680974499</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.45572206176956698</c:v>
+                  <c:v>0.29172984950324599</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.423607965520926</c:v>
+                  <c:v>0.41019367490057707</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.466192529402921</c:v>
+                  <c:v>0.34594980392150204</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.47828012851038099</c:v>
+                  <c:v>0.39692083255552196</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.52057572179401201</c:v>
+                  <c:v>0.25125914730754606</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.41056632111063202</c:v>
+                  <c:v>0.37376195364574905</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.43630146557682797</c:v>
+                  <c:v>0.35649799468618804</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.446945851211624</c:v>
+                  <c:v>0.37931109884962305</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.457451915293831</c:v>
+                  <c:v>0.35983028338178408</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.48583065415085702</c:v>
+                  <c:v>0.30747694127117703</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.38334724327005698</c:v>
+                  <c:v>0.37634131712899299</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.40158398407027701</c:v>
+                  <c:v>0.40631305843067406</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.49157305190433698</c:v>
+                  <c:v>0.34332925299397904</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.420605034401628</c:v>
+                  <c:v>0.34235953504239097</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.45853497471309401</c:v>
+                  <c:v>0.35301900878321202</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.43134459522479002</c:v>
+                  <c:v>0.33281371445927099</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.45222270476099302</c:v>
+                  <c:v>0.37827492524145906</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.43415426904600302</c:v>
+                  <c:v>0.34190265223081501</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -730,7 +1159,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C2D7-4CE0-8187-6A9370F6FBB3}"/>
+              <c16:uniqueId val="{00000000-5412-442D-B50B-273745A91917}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -743,11 +1172,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="500009968"/>
-        <c:axId val="500010624"/>
+        <c:axId val="346477056"/>
+        <c:axId val="346478696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="500009968"/>
+        <c:axId val="346477056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -789,7 +1218,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="500010624"/>
+        <c:crossAx val="346478696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -797,7 +1226,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="500010624"/>
+        <c:axId val="346478696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -848,7 +1277,419 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="500009968"/>
+        <c:crossAx val="346477056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Best - Avg (Survivors)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0.29976029238415203</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.275951462684972</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.29244877277273301</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30419020581258993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.30958987002942195</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.35883762715983708</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.26946696265579195</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.30375600098119099</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.34982904675453402</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.25526143072996993</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.29305665782829299</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.337928504037874</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.30010085790277902</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.29153481696496603</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.26188872727017193</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.29133168686434496</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.35859349437562305</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.36243335619187994</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.24875876870866404</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.38257985467065903</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.30968309654686799</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.25706771797542899</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.267391723263883</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.24819667009222401</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.30087953330898304</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.305473526156264</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.31623827771143903</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.289947782962304</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.29086750705830494</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.36263959689106395</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.299010624916342</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.29116155962368301</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.28427793823043301</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.37639203447907404</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.32380747059707904</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.36171987148961898</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.23942427820598799</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.359433678889368</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.33369853442317204</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.35305414878837604</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.35254808470616905</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.284169345849143</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.35665275672994301</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.39841601592972303</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.28842694809566305</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.31939496559837199</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.33146502528690602</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.31865540477520998</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.34777729523900702</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.335845730953997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5B70-4655-A1F8-E64434D4802E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="414753448"/>
+        <c:axId val="414756400"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="414753448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="414756400"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="414756400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="414753448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -984,6 +1825,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -2016,27 +2897,543 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>162877</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>398145</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>143827</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>464820</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>18097</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>502920</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>952</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1549704D-4376-4DB2-BB11-22ABF9596164}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AF57383-50EA-4708-A031-9F773BF95AB7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2056,23 +3453,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>162877</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>29527</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>636270</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>18097</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>65722</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6FC32F0-11C8-411B-A997-F86B5E9B14A2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F9E97AC-D629-4D0E-9678-2EFB61E4FA51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2085,6 +3482,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>20002</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>56197</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4724176-5635-43B5-9933-40EB12B6DD65}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2356,424 +3789,986 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="29.5234375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.47265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.47265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.3671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>0.37156804283945999</v>
       </c>
       <c r="B2">
         <v>0.38023970761584802</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C2">
+        <v>0.68</v>
+      </c>
+      <c r="E2">
+        <f>C2-A2</f>
+        <v>0.30843195716054006</v>
+      </c>
+      <c r="F2">
+        <f>C2-B2</f>
+        <v>0.29976029238415203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>0.44022145068908503</v>
       </c>
       <c r="B3">
         <v>0.45404853731502798</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C3">
+        <v>0.73</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E51" si="0">C3-A3</f>
+        <v>0.28977854931091496</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F51" si="1">C3-B3</f>
+        <v>0.275951462684972</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>0.425048731023007</v>
       </c>
       <c r="B4">
         <v>0.467551227227267</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C4">
+        <v>0.76</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>0.33495126897699301</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>0.29244877277273301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>0.49638341100141098</v>
       </c>
       <c r="B5">
         <v>0.51580979418741002</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C5">
+        <v>0.82</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.32361658899858897</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>0.30419020581258993</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>0.412818707644731</v>
       </c>
       <c r="B6">
         <v>0.41041012997057802</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C6">
+        <v>0.72</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0.30718129235526898</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>0.30958987002942195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>0.41301451329841099</v>
       </c>
       <c r="B7">
         <v>0.45116237284016297</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C7">
+        <v>0.81</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.39698548670158906</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>0.35883762715983708</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>0.43219416513401598</v>
       </c>
       <c r="B8">
         <v>0.44053303734420801</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C8">
+        <v>0.71</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.27780583486598398</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>0.26946696265579195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>0.437770832926346</v>
       </c>
       <c r="B9">
         <v>0.45624399901880902</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C9">
+        <v>0.76</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0.32222916707365401</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>0.30375600098119099</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>0.41557534736441298</v>
       </c>
       <c r="B10">
         <v>0.44017095324546601</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C10">
+        <v>0.79</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0.37442465263558705</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>0.34982904675453402</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>0.41171546677582499</v>
       </c>
       <c r="B11">
         <v>0.43473856927003002</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C11">
+        <v>0.69</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0.27828453322417496</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>0.25526143072996993</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>0.43937793811444398</v>
       </c>
       <c r="B12">
         <v>0.446943342171707</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C12">
+        <v>0.74</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0.30062206188555601</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>0.29305665782829299</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>0.42207599597787598</v>
       </c>
       <c r="B13">
         <v>0.44207149596212603</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C13">
+        <v>0.78</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>0.35792400402212404</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>0.337928504037874</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>0.458493253303148</v>
       </c>
       <c r="B14">
         <v>0.469899142097221</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C14">
+        <v>0.77</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0.31150674669685202</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>0.30010085790277902</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>0.439251557814899</v>
       </c>
       <c r="B15">
         <v>0.46846518303503398</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C15">
+        <v>0.76</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0.32074844218510101</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>0.29153481696496603</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>0.40786828438216199</v>
       </c>
       <c r="B16">
         <v>0.42811127272982802</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C16">
+        <v>0.69</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>0.28213171561783795</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>0.26188872727017193</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>0.37913904801328102</v>
       </c>
       <c r="B17">
         <v>0.40866831313565499</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C17">
+        <v>0.7</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>0.32086095198671893</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>0.29133168686434496</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>0.42499358252825797</v>
       </c>
       <c r="B18">
         <v>0.45140650562437701</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C18">
+        <v>0.81</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>0.38500641747174208</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>0.35859349437562305</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>0.440720074115035</v>
       </c>
       <c r="B19">
         <v>0.46756664380812002</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C19">
+        <v>0.83</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>0.38927992588496496</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>0.36243335619187994</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>0.38129776129325998</v>
       </c>
       <c r="B20">
         <v>0.411241231291336</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C20">
+        <v>0.66</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>0.27870223870674005</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>0.24875876870866404</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>0.39387563377284401</v>
       </c>
       <c r="B21">
         <v>0.41742014532934102</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C21">
+        <v>0.8</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>0.40612436622715603</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>0.38257985467065903</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>0.42186731023756202</v>
       </c>
       <c r="B22">
         <v>0.430316903453132</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C22">
+        <v>0.74</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>0.31813268976243797</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>0.30968309654686799</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>0.46276402164792602</v>
       </c>
       <c r="B23">
         <v>0.482932282024571</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C23">
+        <v>0.74</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>0.27723597835207398</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>0.25706771797542899</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>0.454262200052099</v>
       </c>
       <c r="B24">
         <v>0.47260827673611699</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C24">
+        <v>0.74</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>0.28573779994790099</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>0.267391723263883</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>0.48053536229008198</v>
       </c>
       <c r="B25">
         <v>0.51180332990777599</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C25">
+        <v>0.76</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>0.27946463770991803</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>0.24819667009222401</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <v>0.47478363719765199</v>
       </c>
       <c r="B26">
         <v>0.489120466691017</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C26">
+        <v>0.79</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>0.31521636280234805</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>0.30087953330898304</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <v>0.42904131551847202</v>
       </c>
       <c r="B27">
         <v>0.46452647384373602</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C27">
+        <v>0.77</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>0.340958684481528</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>0.305473526156264</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <v>0.41967030530504001</v>
       </c>
       <c r="B28">
         <v>0.44376172228856098</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C28">
+        <v>0.76</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>0.34032969469495999</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>0.31623827771143903</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <v>0.45726332462532499</v>
       </c>
       <c r="B29">
         <v>0.460052217037696</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C29">
+        <v>0.75</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>0.29273667537467501</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>0.289947782962304</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
         <v>0.37290103382260498</v>
       </c>
       <c r="B30">
         <v>0.39913249294169501</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C30">
+        <v>0.69</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>0.31709896617739497</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>0.29086750705830494</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
         <v>0.46491658909133998</v>
       </c>
       <c r="B31">
         <v>0.48736040310893602</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C31">
+        <v>0.85</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>0.38508341090866</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>0.36263959689106395</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
         <v>0.430377830880325</v>
       </c>
       <c r="B32">
         <v>0.44098937508365799</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C32">
+        <v>0.74</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>0.30962216911967499</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>0.299010624916342</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
         <v>0.41402019319025501</v>
       </c>
       <c r="B33">
         <v>0.468838440376317</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C33">
+        <v>0.76</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>0.34597980680974499</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>0.29116155962368301</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
         <v>0.44827015049675401</v>
       </c>
       <c r="B34">
         <v>0.45572206176956698</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C34">
+        <v>0.74</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>0.29172984950324599</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>0.28427793823043301</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
         <v>0.38980632509942298</v>
       </c>
       <c r="B35">
         <v>0.423607965520926</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C35">
+        <v>0.8</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>0.41019367490057707</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="1"/>
+        <v>0.37639203447907404</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
         <v>0.44405019607849799</v>
       </c>
       <c r="B36">
         <v>0.466192529402921</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C36">
+        <v>0.79</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>0.34594980392150204</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="1"/>
+        <v>0.32380747059707904</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
         <v>0.44307916744447801</v>
       </c>
       <c r="B37">
         <v>0.47828012851038099</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C37">
+        <v>0.84</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>0.39692083255552196</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="1"/>
+        <v>0.36171987148961898</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
         <v>0.50874085269245395</v>
       </c>
       <c r="B38">
         <v>0.52057572179401201</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C38">
+        <v>0.76</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>0.25125914730754606</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="1"/>
+        <v>0.23942427820598799</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
         <v>0.39623804635425097</v>
       </c>
       <c r="B39">
         <v>0.41056632111063202</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C39">
+        <v>0.77</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>0.37376195364574905</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="1"/>
+        <v>0.359433678889368</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
         <v>0.41350200531381198</v>
       </c>
       <c r="B40">
         <v>0.43630146557682797</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C40">
+        <v>0.77</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="0"/>
+        <v>0.35649799468618804</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="1"/>
+        <v>0.33369853442317204</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
         <v>0.42068890115037699</v>
       </c>
       <c r="B41">
         <v>0.446945851211624</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C41">
+        <v>0.8</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="0"/>
+        <v>0.37931109884962305</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="1"/>
+        <v>0.35305414878837604</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
         <v>0.45016971661821598</v>
       </c>
       <c r="B42">
         <v>0.457451915293831</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C42">
+        <v>0.81</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>0.35983028338178408</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="1"/>
+        <v>0.35254808470616905</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
         <v>0.46252305872882299</v>
       </c>
       <c r="B43">
         <v>0.48583065415085702</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C43">
+        <v>0.77</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>0.30747694127117703</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="1"/>
+        <v>0.284169345849143</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
         <v>0.363658682871007</v>
       </c>
       <c r="B44">
         <v>0.38334724327005698</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C44">
+        <v>0.74</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>0.37634131712899299</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="1"/>
+        <v>0.35665275672994301</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
         <v>0.39368694156932599</v>
       </c>
       <c r="B45">
         <v>0.40158398407027701</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C45">
+        <v>0.8</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>0.40631305843067406</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="1"/>
+        <v>0.39841601592972303</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
         <v>0.43667074700602099</v>
       </c>
       <c r="B46">
         <v>0.49157305190433698</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C46">
+        <v>0.78</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="0"/>
+        <v>0.34332925299397904</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="1"/>
+        <v>0.28842694809566305</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47">
         <v>0.39764046495760902</v>
       </c>
       <c r="B47">
         <v>0.420605034401628</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C47">
+        <v>0.74</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="0"/>
+        <v>0.34235953504239097</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="1"/>
+        <v>0.31939496559837199</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A48">
         <v>0.43698099121678802</v>
       </c>
       <c r="B48">
         <v>0.45853497471309401</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C48">
+        <v>0.79</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="0"/>
+        <v>0.35301900878321202</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="1"/>
+        <v>0.33146502528690602</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A49">
         <v>0.41718628554072901</v>
       </c>
       <c r="B49">
         <v>0.43134459522479002</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C49">
+        <v>0.75</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="0"/>
+        <v>0.33281371445927099</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="1"/>
+        <v>0.31865540477520998</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A50">
         <v>0.42172507475854099</v>
       </c>
       <c r="B50">
         <v>0.45222270476099302</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C50">
+        <v>0.8</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="0"/>
+        <v>0.37827492524145906</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="1"/>
+        <v>0.34777729523900702</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A51">
         <v>0.42809734776918501</v>
       </c>
       <c r="B51">
         <v>0.43415426904600302</v>
+      </c>
+      <c r="C51">
+        <v>0.77</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="0"/>
+        <v>0.34190265223081501</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="1"/>
+        <v>0.335845730953997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>